<commit_message>
cleaning and making plots
</commit_message>
<xml_diff>
--- a/topfill.xlsx
+++ b/topfill.xlsx
@@ -3090,7 +3090,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3120,12 +3120,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -3183,7 +3177,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3206,13 +3200,13 @@
   </sheetPr>
   <dimension ref="A1:O599"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="O293" activeCellId="0" sqref="O293"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.56"/>
@@ -3221,11 +3215,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="5.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="16.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="12.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="16.39"/>
   </cols>

</xml_diff>